<commit_message>
Main Controller PCB Designs
</commit_message>
<xml_diff>
--- a/PCB Design/ElectricalBOM.xlsx
+++ b/PCB Design/ElectricalBOM.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Micah\Documents\School\Masters\ME 495 - RDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB58ACC7-E1BD-4FB6-AAAB-E72DA8924EA5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DBAB8B-5B7E-4F70-8FF7-B327FA788EEF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="624" yWindow="624" windowWidth="17280" windowHeight="9024" activeTab="1" xr2:uid="{3B1A430D-3C31-46ED-B9F8-70FE57591D70}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{3B1A430D-3C31-46ED-B9F8-70FE57591D70}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="WQ Final BOM (NLU)" sheetId="1" r:id="rId1"/>
+    <sheet name="SQ Motor Controller BOM" sheetId="2" r:id="rId2"/>
+    <sheet name="SQ Main Controller BOM" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="167">
   <si>
     <t>Part</t>
   </si>
@@ -487,10 +488,52 @@
     <t>LM2937IMPX-3.3/NOPBCT-ND</t>
   </si>
   <si>
-    <t>micro USB 2.0 receptacle</t>
-  </si>
-  <si>
-    <t>609-4616-1-ND</t>
+    <t>Main Controller</t>
+  </si>
+  <si>
+    <t>C4, C6, C10, C11, C13</t>
+  </si>
+  <si>
+    <t>Needs to change to 120</t>
+  </si>
+  <si>
+    <t>768-1129-1-ND</t>
+  </si>
+  <si>
+    <t>FTDI FT231XS-R</t>
+  </si>
+  <si>
+    <t>CAP 0.1 uF 25V -20/+80 0603</t>
+  </si>
+  <si>
+    <t>399-1100-1-ND</t>
+  </si>
+  <si>
+    <t>CAP 10 uF 16V Tant 1206</t>
+  </si>
+  <si>
+    <t>399-8269-1-ND</t>
+  </si>
+  <si>
+    <t>RES 1 kOhm, 1/10 W, 1%, 0603</t>
+  </si>
+  <si>
+    <t>RMCF0603FT1K00CT-ND</t>
+  </si>
+  <si>
+    <t>microUSB connector</t>
+  </si>
+  <si>
+    <t>609-4613-1-ND</t>
+  </si>
+  <si>
+    <t>296-46360-1-ND</t>
+  </si>
+  <si>
+    <t>C14, C15</t>
+  </si>
+  <si>
+    <t>R10, R11</t>
   </si>
 </sst>
 </file>
@@ -608,7 +651,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -627,13 +670,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -993,14 +1038,14 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
       <c r="M2" t="s">
         <v>80</v>
       </c>
@@ -1730,11 +1775,11 @@
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
       <c r="D26" s="4">
         <f>F25</f>
         <v>21.79</v>
@@ -1905,8 +1950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C17E28D6-48DA-4DE6-8F4D-CB7DF013CEB6}">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1954,14 +1999,14 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
       <c r="M2" t="s">
         <v>80</v>
       </c>
@@ -2040,7 +2085,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" ref="F5:F34" si="0">E5*D5</f>
+        <f t="shared" ref="F5:F33" si="0">E5*D5</f>
         <v>2.0099999999999998</v>
       </c>
       <c r="M5" t="s">
@@ -2864,24 +2909,9 @@
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="D34" s="2">
-        <v>0.45</v>
-      </c>
-      <c r="E34" s="2">
-        <v>1</v>
-      </c>
-      <c r="F34" s="3">
-        <f t="shared" si="0"/>
-        <v>0.45</v>
+      <c r="F34" s="12">
+        <f>SUM(F2:F33)</f>
+        <v>28.98</v>
       </c>
       <c r="M34" t="s">
         <v>123</v>
@@ -2891,10 +2921,6 @@
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F35" s="14">
-        <f>SUM(F2:F34)</f>
-        <v>29.43</v>
-      </c>
       <c r="M35" t="s">
         <v>124</v>
       </c>
@@ -2916,6 +2942,692 @@
       </c>
       <c r="N37">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35B7F842-AEF8-4E46-8FAD-0235FA2637A6}">
+  <dimension ref="A1:H31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" s="3">
+        <v>10.96</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <f>E3*D3</f>
+        <v>10.96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" ref="F4:F29" si="0">E4*D4</f>
+        <v>2.0099999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>6</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" si="0"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="G5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="36" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>3</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="G6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.17</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="0"/>
+        <v>0.17</v>
+      </c>
+      <c r="G8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>2</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="0"/>
+        <v>0.32</v>
+      </c>
+      <c r="G10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>5</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="G12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E13" s="2">
+        <v>2</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>147</v>
+      </c>
+      <c r="H13" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1.82</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="0"/>
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.43</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="0"/>
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" si="0"/>
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E18" s="2">
+        <v>5</v>
+      </c>
+      <c r="F18" s="3">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="G18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.73</v>
+      </c>
+      <c r="E19" s="2">
+        <v>2</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" si="0"/>
+        <v>1.46</v>
+      </c>
+      <c r="G19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E20" s="2">
+        <v>2</v>
+      </c>
+      <c r="F20" s="3">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="G20" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.88</v>
+      </c>
+      <c r="E21" s="2">
+        <v>2</v>
+      </c>
+      <c r="F21" s="3">
+        <f t="shared" si="0"/>
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1.58</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1</v>
+      </c>
+      <c r="F22" s="3">
+        <f t="shared" si="0"/>
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.13</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1</v>
+      </c>
+      <c r="F23" s="3">
+        <f t="shared" si="0"/>
+        <v>0.13</v>
+      </c>
+      <c r="G23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1</v>
+      </c>
+      <c r="F24" s="3">
+        <f t="shared" si="0"/>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="D25" s="16">
+        <v>2.12</v>
+      </c>
+      <c r="E25" s="15">
+        <v>1</v>
+      </c>
+      <c r="F25" s="16">
+        <f t="shared" si="0"/>
+        <v>2.12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="D26" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="E26" s="15">
+        <v>2</v>
+      </c>
+      <c r="F26" s="16">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="G26" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="D27" s="16">
+        <v>0.43</v>
+      </c>
+      <c r="E27" s="15">
+        <v>1</v>
+      </c>
+      <c r="F27" s="16">
+        <f t="shared" si="0"/>
+        <v>0.43</v>
+      </c>
+      <c r="G27" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="D28" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="E28" s="15">
+        <v>2</v>
+      </c>
+      <c r="F28" s="16">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="G28" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="D29" s="16">
+        <v>0.45</v>
+      </c>
+      <c r="E29" s="15">
+        <v>1</v>
+      </c>
+      <c r="F29" s="16">
+        <f t="shared" si="0"/>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F31" s="12">
+        <f>SUM(F2:F30)</f>
+        <v>28.119999999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated BOM to final materials
</commit_message>
<xml_diff>
--- a/PCB Design/ElectricalBOM.xlsx
+++ b/PCB Design/ElectricalBOM.xlsx
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Micah\Documents\GitHub\TBC\PCB Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A08AD06-3544-453A-BF79-5F752E1400F2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFBF5BC-2DB8-4153-AD3A-64184F58BEDD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="7" activeTab="7" xr2:uid="{3B1A430D-3C31-46ED-B9F8-70FE57591D70}"/>
+    <workbookView xWindow="3084" yWindow="3084" windowWidth="17280" windowHeight="9024" firstSheet="5" activeTab="10" xr2:uid="{3B1A430D-3C31-46ED-B9F8-70FE57591D70}"/>
   </bookViews>
   <sheets>
     <sheet name="WQ Final BOM (NLU)" sheetId="1" r:id="rId1"/>
-    <sheet name="SQ Motor Controller v1 BOM" sheetId="2" r:id="rId2"/>
-    <sheet name="SQ Main Controller BOM" sheetId="3" r:id="rId3"/>
-    <sheet name="Full Electrical BOM Ordered" sheetId="6" r:id="rId4"/>
-    <sheet name="Main Controller BOM v1 TP" sheetId="4" r:id="rId5"/>
+    <sheet name="SQ Motor Controller v1 (NLU)" sheetId="2" r:id="rId2"/>
+    <sheet name="SQ Main Controller (NLU)" sheetId="3" r:id="rId3"/>
+    <sheet name="Full v1 Electrical BOM Ordered" sheetId="6" r:id="rId4"/>
+    <sheet name="Main Controller v1 TP" sheetId="4" r:id="rId5"/>
     <sheet name="SQ Motor Controller v2 BOM" sheetId="7" r:id="rId6"/>
     <sheet name="SQ Main Controller v2 BOM" sheetId="8" r:id="rId7"/>
     <sheet name="Encoder BOM" sheetId="5" r:id="rId8"/>
+    <sheet name="v2 Boards TP" sheetId="9" r:id="rId9"/>
+    <sheet name="Wires" sheetId="10" r:id="rId10"/>
+    <sheet name="Misc." sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="240">
   <si>
     <t>Part</t>
   </si>
@@ -671,6 +674,93 @@
   </si>
   <si>
     <t>455-1163-ND</t>
+  </si>
+  <si>
+    <t>Prowire USA</t>
+  </si>
+  <si>
+    <t>20 AWG x 2 Shielded Cable</t>
+  </si>
+  <si>
+    <t>M27500/20SB2T23</t>
+  </si>
+  <si>
+    <t>20 AWG Red Wire</t>
+  </si>
+  <si>
+    <t>20 AWG Black Wire</t>
+  </si>
+  <si>
+    <t>M22759/32-20-2</t>
+  </si>
+  <si>
+    <t>M22759/32-20-0</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>DR-25-1/8-0-UK</t>
+  </si>
+  <si>
+    <t>1/8" Tubing</t>
+  </si>
+  <si>
+    <t>22 AWG 6 cable</t>
+  </si>
+  <si>
+    <t>1176C SL005</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://prowireusa.com/p-1665-22-awg-x-6-non-shielded-cable.aspx</t>
+  </si>
+  <si>
+    <t>Shield Terminator</t>
+  </si>
+  <si>
+    <t>S02-07-R</t>
+  </si>
+  <si>
+    <t>https://prowireusa.com/p-1088-shield-terminator-with-22-gauge-lead.aspx</t>
+  </si>
+  <si>
+    <t>https://prowireusa.com/p-1291-dr-25-1-8-tubing-white-print.aspx</t>
+  </si>
+  <si>
+    <t>https://prowireusa.com/p-565-m22759-32-20-2-red-wire-tefzel-20-awg.aspx</t>
+  </si>
+  <si>
+    <t>https://prowireusa.com/p-566-m22759-32-20-0-black-wire-tefzel-20-awg.aspx</t>
+  </si>
+  <si>
+    <t>https://prowireusa.com/p-2148-20-awg-x-2-shielded-cable.aspx</t>
+  </si>
+  <si>
+    <t>F4193-ND</t>
+  </si>
+  <si>
+    <t>486-2246-ND</t>
+  </si>
+  <si>
+    <t>Encoder IC</t>
+  </si>
+  <si>
+    <t>5-pin header</t>
+  </si>
+  <si>
+    <t>5-pin connector</t>
+  </si>
+  <si>
+    <t>3A Fuse</t>
+  </si>
+  <si>
+    <t>PWR Switch</t>
   </si>
 </sst>
 </file>
@@ -680,7 +770,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -716,6 +806,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -725,7 +823,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -820,12 +918,171 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -869,6 +1126,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -881,12 +1170,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1205,15 +1507,15 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1242,15 +1544,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
       <c r="M2" t="s">
         <v>80</v>
       </c>
@@ -1261,7 +1563,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1291,7 +1593,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -1321,7 +1623,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>31</v>
       </c>
@@ -1351,7 +1653,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>69</v>
       </c>
@@ -1384,7 +1686,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>36</v>
       </c>
@@ -1417,7 +1719,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>63</v>
       </c>
@@ -1450,7 +1752,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>66</v>
       </c>
@@ -1483,7 +1785,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -1516,7 +1818,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -1546,7 +1848,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>39</v>
       </c>
@@ -1579,7 +1881,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>55</v>
       </c>
@@ -1612,7 +1914,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>44</v>
       </c>
@@ -1645,7 +1947,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>32</v>
       </c>
@@ -1678,7 +1980,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>33</v>
       </c>
@@ -1711,7 +2013,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>47</v>
       </c>
@@ -1744,7 +2046,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>49</v>
       </c>
@@ -1777,7 +2079,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>51</v>
       </c>
@@ -1810,7 +2112,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
@@ -1843,7 +2145,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
@@ -1873,7 +2175,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>15</v>
       </c>
@@ -1903,7 +2205,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
@@ -1933,7 +2235,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>17</v>
       </c>
@@ -1963,7 +2265,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D25" s="4"/>
       <c r="F25" s="4">
         <f>SUM(F3:F24)</f>
@@ -1979,12 +2281,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A26" s="26" t="s">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
+      <c r="B26" s="52"/>
+      <c r="C26" s="52"/>
       <c r="D26" s="4">
         <f>F25</f>
         <v>21.79</v>
@@ -2006,7 +2308,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
@@ -2014,7 +2316,7 @@
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
@@ -2022,7 +2324,7 @@
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -2039,7 +2341,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>57</v>
       </c>
@@ -2056,7 +2358,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>59</v>
       </c>
@@ -2073,7 +2375,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>61</v>
       </c>
@@ -2090,7 +2392,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>72</v>
       </c>
@@ -2107,7 +2409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>74</v>
       </c>
@@ -2124,7 +2426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>76</v>
       </c>
@@ -2148,6 +2450,369 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52AB6D92-77D5-463B-8F87-D30E3BA4597A}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="67.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="48" t="s">
+        <v>218</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="48" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="F2" s="2">
+        <v>20</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2*E2</f>
+        <v>12.7</v>
+      </c>
+      <c r="H2" s="49" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D3" s="2">
+        <v>25</v>
+      </c>
+      <c r="E3" s="3">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3" si="0">F3*E3</f>
+        <v>8</v>
+      </c>
+      <c r="H3" s="49" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D4" s="2">
+        <v>25</v>
+      </c>
+      <c r="E4" s="3">
+        <v>8</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <f>F4*E4</f>
+        <v>8</v>
+      </c>
+      <c r="H4" s="49" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E5" s="14">
+        <v>2.048</v>
+      </c>
+      <c r="F5" s="2">
+        <v>10</v>
+      </c>
+      <c r="G5" s="3">
+        <f>F5*E5</f>
+        <v>20.48</v>
+      </c>
+      <c r="H5" s="50" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F6" s="2">
+        <v>5</v>
+      </c>
+      <c r="G6" s="14">
+        <f>F6*E6</f>
+        <v>2.8499999999999996</v>
+      </c>
+      <c r="H6" s="50" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E7" s="14">
+        <v>1.25</v>
+      </c>
+      <c r="F7" s="2">
+        <v>10</v>
+      </c>
+      <c r="G7" s="14">
+        <f>F7*E7</f>
+        <v>12.5</v>
+      </c>
+      <c r="H7" s="50" t="s">
+        <v>228</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H7" r:id="rId1" xr:uid="{B44C77A2-10A6-4E1A-8C64-CFD3E6AD9AE4}"/>
+    <hyperlink ref="H5" r:id="rId2" xr:uid="{86EDA71A-0E8E-44D7-B002-AC2CD77DE550}"/>
+    <hyperlink ref="H3" r:id="rId3" xr:uid="{CD3BA3CF-3155-45E4-B0DB-5A7CE1C52F17}"/>
+    <hyperlink ref="H4" r:id="rId4" xr:uid="{F3347143-8BBC-4BBC-A21B-E0213324EB62}"/>
+    <hyperlink ref="H2" r:id="rId5" xr:uid="{5B73DBD6-65FD-4660-B2E2-86B3E970F888}"/>
+    <hyperlink ref="H6" r:id="rId6" xr:uid="{4CE9C536-6C4B-4560-9A66-73EEE673C60C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7074AEB1-32CC-4224-BBE2-72D2E92A2D3D}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="D2" s="3">
+        <v>11.936</v>
+      </c>
+      <c r="E2" s="23">
+        <v>6</v>
+      </c>
+      <c r="F2" s="27">
+        <f>E2*D2</f>
+        <v>71.616</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.27</v>
+      </c>
+      <c r="E3" s="2">
+        <v>6</v>
+      </c>
+      <c r="F3" s="27">
+        <f t="shared" ref="F3:F6" si="0">E3*D3</f>
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="E4" s="2">
+        <v>6</v>
+      </c>
+      <c r="F4" s="27">
+        <f t="shared" si="0"/>
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="E5" s="2">
+        <v>6</v>
+      </c>
+      <c r="F5" s="27">
+        <f t="shared" si="0"/>
+        <v>1.6320000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="D6" s="3">
+        <v>14.89</v>
+      </c>
+      <c r="E6" s="13">
+        <v>1</v>
+      </c>
+      <c r="F6" s="27">
+        <f t="shared" si="0"/>
+        <v>14.89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2159,22 +2824,22 @@
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2203,15 +2868,15 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
       <c r="M2" t="s">
         <v>80</v>
       </c>
@@ -2219,7 +2884,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -2246,7 +2911,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -2273,7 +2938,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>31</v>
       </c>
@@ -2300,7 +2965,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>69</v>
       </c>
@@ -2330,7 +2995,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>36</v>
       </c>
@@ -2360,7 +3025,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>63</v>
       </c>
@@ -2390,7 +3055,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>66</v>
       </c>
@@ -2420,7 +3085,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -2450,7 +3115,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>18</v>
       </c>
@@ -2480,7 +3145,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>39</v>
       </c>
@@ -2510,7 +3175,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>55</v>
       </c>
@@ -2540,7 +3205,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>44</v>
       </c>
@@ -2570,7 +3235,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>32</v>
       </c>
@@ -2600,7 +3265,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>33</v>
       </c>
@@ -2630,7 +3295,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>47</v>
       </c>
@@ -2660,7 +3325,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>49</v>
       </c>
@@ -2690,7 +3355,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>51</v>
       </c>
@@ -2720,7 +3385,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
@@ -2750,7 +3415,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
@@ -2777,7 +3442,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>15</v>
       </c>
@@ -2804,7 +3469,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
@@ -2831,7 +3496,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>17</v>
       </c>
@@ -2858,7 +3523,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>53</v>
       </c>
@@ -2888,7 +3553,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>57</v>
       </c>
@@ -2918,7 +3583,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>59</v>
       </c>
@@ -2948,7 +3613,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>61</v>
       </c>
@@ -2969,7 +3634,7 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>72</v>
       </c>
@@ -2999,7 +3664,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>74</v>
       </c>
@@ -3026,7 +3691,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>76</v>
       </c>
@@ -3053,7 +3718,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>138</v>
       </c>
@@ -3083,7 +3748,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>140</v>
       </c>
@@ -3113,7 +3778,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F34" s="12">
         <f>SUM(F2:F33)</f>
         <v>28.98</v>
@@ -3125,7 +3790,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M35" t="s">
         <v>124</v>
       </c>
@@ -3133,7 +3798,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M36" t="s">
         <v>125</v>
       </c>
@@ -3141,7 +3806,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M37" t="s">
         <v>126</v>
       </c>
@@ -3165,17 +3830,17 @@
       <selection activeCell="G31" sqref="A1:G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3198,17 +3863,17 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="51" t="s">
         <v>151</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -3229,7 +3894,7 @@
         <v>10.96</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>31</v>
       </c>
@@ -3250,7 +3915,7 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>36</v>
       </c>
@@ -3274,7 +3939,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>39</v>
       </c>
@@ -3298,7 +3963,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>55</v>
       </c>
@@ -3322,7 +3987,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>44</v>
       </c>
@@ -3346,7 +4011,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
@@ -3370,7 +4035,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>33</v>
       </c>
@@ -3394,7 +4059,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>47</v>
       </c>
@@ -3418,7 +4083,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>49</v>
       </c>
@@ -3442,7 +4107,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -3469,7 +4134,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -3490,7 +4155,7 @@
         <v>1.82</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -3511,7 +4176,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -3532,7 +4197,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -3553,7 +4218,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>53</v>
       </c>
@@ -3577,7 +4242,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>57</v>
       </c>
@@ -3601,7 +4266,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>59</v>
       </c>
@@ -3625,7 +4290,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>61</v>
       </c>
@@ -3646,7 +4311,7 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>74</v>
       </c>
@@ -3667,7 +4332,7 @@
         <v>1.58</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>138</v>
       </c>
@@ -3691,7 +4356,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>140</v>
       </c>
@@ -3715,7 +4380,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>155</v>
       </c>
@@ -3736,7 +4401,7 @@
         <v>2.12</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>156</v>
       </c>
@@ -3760,7 +4425,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>158</v>
       </c>
@@ -3784,7 +4449,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>160</v>
       </c>
@@ -3808,7 +4473,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>162</v>
       </c>
@@ -3829,7 +4494,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F31" s="12">
         <f>SUM(F2:F30)</f>
         <v>28.119999999999994</v>
@@ -3849,20 +4514,20 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3882,7 +4547,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -3903,7 +4568,7 @@
         <v>38.4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>170</v>
       </c>
@@ -3924,7 +4589,7 @@
         <v>78.099999999999994</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>31</v>
       </c>
@@ -3945,7 +4610,7 @@
         <v>20.099999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>69</v>
       </c>
@@ -3966,7 +4631,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>36</v>
       </c>
@@ -3987,7 +4652,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>63</v>
       </c>
@@ -4008,7 +4673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>66</v>
       </c>
@@ -4029,7 +4694,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -4050,7 +4715,7 @@
         <v>3.4000000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>18</v>
       </c>
@@ -4071,7 +4736,7 @@
         <v>9.75</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>39</v>
       </c>
@@ -4092,7 +4757,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>55</v>
       </c>
@@ -4113,7 +4778,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>44</v>
       </c>
@@ -4134,7 +4799,7 @@
         <v>1.7000000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>32</v>
       </c>
@@ -4155,7 +4820,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>33</v>
       </c>
@@ -4176,7 +4841,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>47</v>
       </c>
@@ -4197,7 +4862,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>49</v>
       </c>
@@ -4218,7 +4883,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>51</v>
       </c>
@@ -4239,7 +4904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>13</v>
       </c>
@@ -4260,7 +4925,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -4281,7 +4946,7 @@
         <v>18.2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
@@ -4302,7 +4967,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
@@ -4323,7 +4988,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>17</v>
       </c>
@@ -4344,7 +5009,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>53</v>
       </c>
@@ -4365,7 +5030,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>57</v>
       </c>
@@ -4386,7 +5051,7 @@
         <v>18.25</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>59</v>
       </c>
@@ -4407,7 +5072,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>61</v>
       </c>
@@ -4428,7 +5093,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>72</v>
       </c>
@@ -4449,7 +5114,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>74</v>
       </c>
@@ -4470,7 +5135,7 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>76</v>
       </c>
@@ -4491,7 +5156,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>138</v>
       </c>
@@ -4512,7 +5177,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>140</v>
       </c>
@@ -4533,7 +5198,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>10</v>
       </c>
@@ -4554,7 +5219,7 @@
         <v>54.800000000000004</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>155</v>
       </c>
@@ -4575,7 +5240,7 @@
         <v>4.24</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>156</v>
       </c>
@@ -4596,7 +5261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>158</v>
       </c>
@@ -4617,7 +5282,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>160</v>
       </c>
@@ -4638,7 +5303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>162</v>
       </c>
@@ -4659,7 +5324,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>171</v>
       </c>
@@ -4680,7 +5345,7 @@
         <v>71.89</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>173</v>
       </c>
@@ -4701,7 +5366,7 @@
         <v>11.11</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F41" s="12">
         <f>SUM(F2:F40)</f>
         <v>466.49999999999994</v>
@@ -4717,28 +5382,28 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="53" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="E1" s="25" t="s">
+      <c r="B1" s="54"/>
+      <c r="E1" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="25"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F1" s="51"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
@@ -4752,7 +5417,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>10</v>
       </c>
@@ -4762,7 +5427,7 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>31</v>
       </c>
@@ -4772,7 +5437,7 @@
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>36</v>
       </c>
@@ -4784,7 +5449,7 @@
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>39</v>
       </c>
@@ -4798,7 +5463,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>55</v>
       </c>
@@ -4812,7 +5477,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>44</v>
       </c>
@@ -4826,7 +5491,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>32</v>
       </c>
@@ -4840,7 +5505,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>33</v>
       </c>
@@ -4854,7 +5519,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>47</v>
       </c>
@@ -4868,7 +5533,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>49</v>
       </c>
@@ -4882,7 +5547,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>13</v>
       </c>
@@ -4896,7 +5561,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>14</v>
       </c>
@@ -4908,7 +5573,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>15</v>
       </c>
@@ -4920,7 +5585,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>16</v>
       </c>
@@ -4932,7 +5597,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>17</v>
       </c>
@@ -4944,7 +5609,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>53</v>
       </c>
@@ -4958,7 +5623,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>57</v>
       </c>
@@ -4972,7 +5637,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>59</v>
       </c>
@@ -4986,7 +5651,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>61</v>
       </c>
@@ -4996,7 +5661,7 @@
       </c>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>74</v>
       </c>
@@ -5006,7 +5671,7 @@
       </c>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>138</v>
       </c>
@@ -5018,7 +5683,7 @@
       </c>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>140</v>
       </c>
@@ -5030,7 +5695,7 @@
       </c>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>155</v>
       </c>
@@ -5042,7 +5707,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
         <v>156</v>
       </c>
@@ -5056,7 +5721,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
         <v>158</v>
       </c>
@@ -5070,7 +5735,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>160</v>
       </c>
@@ -5082,7 +5747,7 @@
       </c>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>162</v>
       </c>
@@ -5094,19 +5759,19 @@
         <v>130</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E30" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E31" s="2" t="s">
         <v>76</v>
       </c>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E32" s="2" t="s">
         <v>138</v>
       </c>
@@ -5114,7 +5779,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E33" s="2" t="s">
         <v>140</v>
       </c>
@@ -5137,21 +5802,21 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F41" sqref="A3:F41"/>
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5174,17 +5839,17 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -5205,7 +5870,7 @@
         <v>3.84</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -5226,7 +5891,7 @@
         <v>10.96</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>31</v>
       </c>
@@ -5247,7 +5912,7 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>69</v>
       </c>
@@ -5271,7 +5936,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>36</v>
       </c>
@@ -5295,7 +5960,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>63</v>
       </c>
@@ -5319,7 +5984,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>66</v>
       </c>
@@ -5343,7 +6008,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -5367,7 +6032,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>18</v>
       </c>
@@ -5391,7 +6056,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>39</v>
       </c>
@@ -5415,7 +6080,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>55</v>
       </c>
@@ -5439,7 +6104,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>44</v>
       </c>
@@ -5463,7 +6128,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>32</v>
       </c>
@@ -5487,7 +6152,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>33</v>
       </c>
@@ -5511,7 +6176,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>47</v>
       </c>
@@ -5535,7 +6200,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>49</v>
       </c>
@@ -5559,7 +6224,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>51</v>
       </c>
@@ -5583,7 +6248,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -5604,7 +6269,7 @@
         <v>1.82</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
@@ -5625,7 +6290,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
@@ -5646,7 +6311,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>17</v>
       </c>
@@ -5667,7 +6332,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>53</v>
       </c>
@@ -5691,7 +6356,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>57</v>
       </c>
@@ -5715,7 +6380,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>179</v>
       </c>
@@ -5739,7 +6404,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>181</v>
       </c>
@@ -5756,14 +6421,14 @@
         <v>1</v>
       </c>
       <c r="F27" s="3">
-        <f>E27*D27</f>
+        <f t="shared" ref="F27:F41" si="1">E27*D27</f>
         <v>0.35</v>
       </c>
       <c r="G27" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>138</v>
       </c>
@@ -5780,14 +6445,14 @@
         <v>1</v>
       </c>
       <c r="F28" s="3">
-        <f>E28*D28</f>
+        <f t="shared" si="1"/>
         <v>0.13</v>
       </c>
       <c r="G28" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>140</v>
       </c>
@@ -5804,21 +6469,21 @@
         <v>1</v>
       </c>
       <c r="F29" s="3">
-        <f>E29*D29</f>
+        <f t="shared" si="1"/>
         <v>0.28999999999999998</v>
       </c>
       <c r="G29" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>185</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="29" t="s">
+      <c r="C30" s="25" t="s">
         <v>175</v>
       </c>
       <c r="D30" s="3">
@@ -5828,11 +6493,11 @@
         <v>2</v>
       </c>
       <c r="F30" s="3">
-        <f>E30*D30</f>
+        <f t="shared" si="1"/>
         <v>0.34</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>186</v>
       </c>
@@ -5849,11 +6514,11 @@
         <v>1</v>
       </c>
       <c r="F31" s="3">
-        <f>E31*D31</f>
+        <f t="shared" si="1"/>
         <v>0.22</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>187</v>
       </c>
@@ -5870,11 +6535,11 @@
         <v>1</v>
       </c>
       <c r="F32" s="3">
-        <f>E32*D32</f>
+        <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>188</v>
       </c>
@@ -5891,11 +6556,11 @@
         <v>1</v>
       </c>
       <c r="F33" s="3">
-        <f>E33*D33</f>
+        <f t="shared" si="1"/>
         <v>0.34</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>189</v>
       </c>
@@ -5912,11 +6577,11 @@
         <v>2</v>
       </c>
       <c r="F34" s="3">
-        <f>E34*D34</f>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>190</v>
       </c>
@@ -5933,11 +6598,11 @@
         <v>1</v>
       </c>
       <c r="F35" s="3">
-        <f>E35*D35</f>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>191</v>
       </c>
@@ -5954,11 +6619,11 @@
         <v>1</v>
       </c>
       <c r="F36" s="3">
-        <f>E36*D36</f>
+        <f t="shared" si="1"/>
         <v>0.12</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>192</v>
       </c>
@@ -5975,11 +6640,11 @@
         <v>1</v>
       </c>
       <c r="F37" s="3">
-        <f>E37*D37</f>
+        <f t="shared" si="1"/>
         <v>0.15</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>193</v>
       </c>
@@ -5996,11 +6661,11 @@
         <v>20</v>
       </c>
       <c r="F38" s="3">
-        <f>E38*D38</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>199</v>
       </c>
@@ -6017,11 +6682,11 @@
         <v>5</v>
       </c>
       <c r="F39" s="14">
-        <f>E39*D39</f>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>201</v>
       </c>
@@ -6038,11 +6703,11 @@
         <v>1</v>
       </c>
       <c r="F40" s="14">
-        <f>E40*D40</f>
+        <f t="shared" si="1"/>
         <v>1.03</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>203</v>
       </c>
@@ -6059,11 +6724,11 @@
         <v>1</v>
       </c>
       <c r="F41" s="14">
-        <f>E41*D41</f>
+        <f t="shared" si="1"/>
         <v>1.33</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F42" s="12">
         <f>SUM(F2:F41)</f>
         <v>33.830000000000005</v>
@@ -6082,22 +6747,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A80F09-CA95-4E8A-AF30-A3533B50B548}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="A3:F32"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6120,17 +6785,17 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="51" t="s">
         <v>151</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -6151,7 +6816,7 @@
         <v>10.96</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>31</v>
       </c>
@@ -6172,7 +6837,7 @@
         <v>4.0199999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>36</v>
       </c>
@@ -6196,7 +6861,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>39</v>
       </c>
@@ -6220,7 +6885,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>55</v>
       </c>
@@ -6244,7 +6909,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>44</v>
       </c>
@@ -6268,7 +6933,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
@@ -6292,7 +6957,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>33</v>
       </c>
@@ -6316,7 +6981,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>47</v>
       </c>
@@ -6340,7 +7005,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>49</v>
       </c>
@@ -6364,7 +7029,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
@@ -6385,7 +7050,7 @@
         <v>1.82</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -6406,7 +7071,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
@@ -6427,7 +7092,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
@@ -6448,7 +7113,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>53</v>
       </c>
@@ -6472,7 +7137,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>57</v>
       </c>
@@ -6496,7 +7161,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>138</v>
       </c>
@@ -6520,7 +7185,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>140</v>
       </c>
@@ -6544,7 +7209,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>155</v>
       </c>
@@ -6565,7 +7230,7 @@
         <v>2.12</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>156</v>
       </c>
@@ -6589,7 +7254,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>158</v>
       </c>
@@ -6613,7 +7278,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>160</v>
       </c>
@@ -6637,7 +7302,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>162</v>
       </c>
@@ -6658,14 +7323,14 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>185</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="29" t="s">
+      <c r="C26" s="25" t="s">
         <v>175</v>
       </c>
       <c r="D26" s="3">
@@ -6675,11 +7340,11 @@
         <v>4</v>
       </c>
       <c r="F26" s="3">
-        <f>E26*D26</f>
+        <f t="shared" ref="F26:F32" si="1">E26*D26</f>
         <v>0.68</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>187</v>
       </c>
@@ -6696,11 +7361,11 @@
         <v>1</v>
       </c>
       <c r="F27" s="3">
-        <f>E27*D27</f>
+        <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>189</v>
       </c>
@@ -6717,11 +7382,11 @@
         <v>4</v>
       </c>
       <c r="F28" s="3">
-        <f>E28*D28</f>
+        <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>191</v>
       </c>
@@ -6738,11 +7403,11 @@
         <v>1</v>
       </c>
       <c r="F29" s="3">
-        <f>E29*D29</f>
+        <f t="shared" si="1"/>
         <v>0.12</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>199</v>
       </c>
@@ -6759,11 +7424,11 @@
         <v>10</v>
       </c>
       <c r="F30" s="14">
-        <f>E30*D30</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>193</v>
       </c>
@@ -6780,18 +7445,18 @@
         <v>10</v>
       </c>
       <c r="F31" s="3">
-        <f>E31*D31</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>206</v>
       </c>
       <c r="B32" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="30" t="s">
+      <c r="C32" s="26" t="s">
         <v>205</v>
       </c>
       <c r="D32" s="14">
@@ -6801,11 +7466,11 @@
         <v>1</v>
       </c>
       <c r="F32" s="14">
-        <f>E32*D32</f>
+        <f t="shared" si="1"/>
         <v>2.2400000000000002</v>
       </c>
     </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F34" s="12">
         <f>SUM(F2:F26)</f>
         <v>28.529999999999998</v>
@@ -6823,21 +7488,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF56E153-847C-4A14-9D26-792BACCDDC08}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6857,17 +7522,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="51" t="s">
         <v>167</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>168</v>
       </c>
@@ -6888,7 +7553,7 @@
         <v>13.61</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>36</v>
       </c>
@@ -6909,7 +7574,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>49</v>
       </c>
@@ -6930,7 +7595,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -6951,7 +7616,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>53</v>
       </c>
@@ -6972,7 +7637,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>207</v>
       </c>
@@ -6993,7 +7658,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>209</v>
       </c>
@@ -7009,12 +7674,12 @@
       <c r="E9" s="2">
         <v>1</v>
       </c>
-      <c r="F9" s="31">
+      <c r="F9" s="27">
         <f>E9*D9</f>
         <v>0.11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>193</v>
       </c>
@@ -7035,7 +7700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F11" s="12">
         <f>SUM(F2:F10)</f>
         <v>16.069999999999997</v>
@@ -7048,4 +7713,795 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F7D0B46-AD6F-4CDE-9C68-9EE642CFEC41}">
+  <dimension ref="A1:I40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="55" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="56"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="58" t="s">
+        <v>151</v>
+      </c>
+      <c r="E1" s="58"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="39"/>
+      <c r="D2" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F2" s="39"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="30"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" s="39"/>
+      <c r="D3" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="39"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="30"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="39"/>
+      <c r="D4" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="G4" s="30"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="30"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="G5" s="30"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="30"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="G6" s="30"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="30"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="G7" s="30"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="30"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>144</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="G8" s="30"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="30"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="30"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="30"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="G10" s="30"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="30"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="39" t="s">
+        <v>148</v>
+      </c>
+      <c r="G11" s="30"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="30"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F12" s="39"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="30"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="39"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="30"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="39"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="30"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="39"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="30"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="G16" s="30"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="30"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="39" t="s">
+        <v>148</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="G17" s="30"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="30"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="39" t="s">
+        <v>146</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F18" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="G18" s="30"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="30"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C19" s="39"/>
+      <c r="D19" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F19" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="G19" s="30"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="30"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="39"/>
+      <c r="D20" s="37" t="s">
+        <v>155</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="F20" s="39"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="31"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="39"/>
+      <c r="D21" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="F21" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="G21" s="31"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="31"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="39"/>
+      <c r="D22" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="F22" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="G22" s="31"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="31"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="D23" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="F23" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="G23" s="31"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="31"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="D24" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="F24" s="39"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="31"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="38" t="s">
+        <v>179</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C25" s="39" t="s">
+        <v>183</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>185</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="F25" s="39"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="30"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="38" t="s">
+        <v>181</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C26" s="39" t="s">
+        <v>184</v>
+      </c>
+      <c r="D26" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F26" s="39"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="30"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C27" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F27" s="39"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="30"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="38" t="s">
+        <v>140</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C28" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F28" s="39"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="30"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="38" t="s">
+        <v>185</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="C29" s="39"/>
+      <c r="D29" s="37" t="s">
+        <v>199</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="F29" s="39"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="31"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="38" t="s">
+        <v>186</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C30" s="39"/>
+      <c r="D30" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F30" s="39"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="30"/>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="C31" s="39"/>
+      <c r="D31" s="47" t="s">
+        <v>206</v>
+      </c>
+      <c r="E31" s="45" t="s">
+        <v>205</v>
+      </c>
+      <c r="F31" s="46"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="31"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="38" t="s">
+        <v>188</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="C32" s="39"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="30"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="42" t="s">
+        <v>189</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="C33" s="39"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="30"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="C34" s="39"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="30"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="42" t="s">
+        <v>191</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="C35" s="39"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="30"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="42" t="s">
+        <v>192</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="C36" s="39"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="30"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="42" t="s">
+        <v>193</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="C37" s="39"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="30"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="C38" s="39"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="31"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="42" t="s">
+        <v>201</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="C39" s="39"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="31"/>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="43" t="s">
+        <v>203</v>
+      </c>
+      <c r="B40" s="44" t="s">
+        <v>204</v>
+      </c>
+      <c r="C40" s="46"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="31"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>